<commit_message>
6eme changement. Règle N°131. Ajout d'attribut pour les liens. (Label). Plus modification intitulé de la page 2. Transformé en Formulaire-de-Contact. Modification liens page Index. En liens twitter-facebook-Dribble-Instagram.
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -19,194 +19,8 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="61">
-  <si>
-    <t xml:space="preserve">Catégorie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Problème identifié</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Explication du problème</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bonne pratique à adopter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Action recommandée</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Référence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Présentation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contraste de la page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Problèmes de contraste entre le texte et l’arrière plan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Un ratio de contraste minimal de 3:1 entre le texte et son arrière-plan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://checklists.opquast.com/fr/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Langue page2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">          Langue / défaut </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Mettre la langue VF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cours </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Structure-Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Meta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Meta /obsolete </t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Enlever la méta keywords</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Title sans de valeur Page principale et « page 2 » pour la seconde page.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mettre des mots clefs qui correspondent 
-Au sujet principal du site 70 caractères maximum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cours</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Meta description sans de valeur.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Mettre entre  70 -320 caractères </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> .  HREF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Chemin local pour les valeur Href  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mettre des chemins relatifs </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.alsacreations.com/astuce/lire/78-Quelle-est-la-difference-entre-les-chemins-relatifs-et-absolus-.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    http://www.php-astux.info/chemins-relatif-absolu.php</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CSS balise style</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pas de précence d’aria dans les pages</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mettre des ARIA pour les personnes handicapés</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  URL </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  URL pas adapté</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Mettre une adresse URL adapté au sujet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Image et média</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Répétition ALT  IMG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Répétition dans les attributs  des images</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mettre des Alt différents (éviter les spams)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Format d’image</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mauvais format d’image bmp ( trop lourde)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Format JPEG ou PeG ou GIF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Texte en image</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Du texte présent dans une balise img</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ne jamais mettre de texte dans une balise img</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Formulaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Annuaire -Liste</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Liste annuaire mal construite et spam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ne plus faire d’annuaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Navigation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Les titres h1-h2-h3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Titre pas dans l’ordre H3 avant h2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mettre les titres dans l’ordre h1-h2 -h3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Security</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Liens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identification et contact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Données personnalisés</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Serveur et performance</t>
-  </si>
-</sst>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="UTF-8" standalone="yes"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="69"><si><t xml:space="preserve">Catégorie</t></si><si><t xml:space="preserve">Problème identifié</t></si><si><t xml:space="preserve">Explication du problème</t></si><si><t xml:space="preserve">Bonne pratique à adopter</t></si><si><t xml:space="preserve">Action recommandée</t></si><si><t xml:space="preserve">Référence</t></si><si><t xml:space="preserve">Présentation</t></si><si><t xml:space="preserve">Contraste de la page</t></si><si><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">Problèmes de contraste entre le texte et l’arrière plan</t></r><r><rPr><b val="true"/><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">(accessibilité)</t></r></si><si><t xml:space="preserve">Un ratio de contraste minimal de 3:1 entre le texte et son arrière-plan</t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°177</t></si><si><t xml:space="preserve">Langue page2</t></si><si><t xml:space="preserve">          Langue / défaut </t></si><si><t xml:space="preserve">  Mettre la langue VF</t></si><si><t xml:space="preserve">Cours </t></si><si><t xml:space="preserve">Structure-Code</t></si><si><t xml:space="preserve">Meta</t></si><si><t xml:space="preserve">  Meta /obsolete </t></si><si><t xml:space="preserve">    Enlever la méta keywords</t></si><si><t xml:space="preserve"> Title sans de valeur Page principale et « page 2 » pour la seconde page.</t></si><si><t xml:space="preserve"> Mettre des mots clefs qui correspondent &#10;Au sujet principal du site 70 caractères maximum</t></si><si><t xml:space="preserve">&#10;</t></si><si><t xml:space="preserve">Cours</t></si><si><t xml:space="preserve"> Meta description sans de valeur.</t></si><si><t xml:space="preserve">  Mettre entre  70 -320 caractères </t></si><si><t xml:space="preserve">https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html</t></si><si><t xml:space="preserve"> .  HREF</t></si><si><t xml:space="preserve">   Chemin local pour les valeur Href  </t></si><si><t xml:space="preserve"> Mettre des chemins relatifs </t></si><si><t xml:space="preserve">https://www.alsacreations.com/astuce/lire/78-Quelle-est-la-difference-entre-les-chemins-relatifs-et-absolus-.html</t></si><si><t xml:space="preserve">    http://www.php-astux.info/chemins-relatif-absolu.php</t></si><si><t xml:space="preserve"> CSS balise style</t></si><si><t xml:space="preserve"> Pas de précence d’aria dans les pages</t></si><si><t xml:space="preserve"> Mettre des ARIA pour les personnes handicapés</t></si><si><t xml:space="preserve">  URL </t></si><si><t xml:space="preserve">  URL pas adapté</t></si><si><t xml:space="preserve">  Mettre une adresse URL adapté au sujet</t></si><si><t xml:space="preserve">Image et média</t></si><si><t xml:space="preserve">Répétition ALT  IMG</t></si><si><t xml:space="preserve">  Répétition dans les attributs  des images</t></si><si><t xml:space="preserve"> Mettre des Alt différents (éviter les spams)</t></si><si><t xml:space="preserve"> Cours</t></si><si><t xml:space="preserve">Format d’image</t></si><si><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/></rPr><t xml:space="preserve">Mauvais format d’image bmp  trop lourde +6Mo.</t></r><r><rPr><b val="true"/><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/></rPr><t xml:space="preserve"> ( Vitesse et taille du site )</t></r></si><si><t xml:space="preserve">Format JPEG ou PeG ou GIF</t></si><si><t xml:space="preserve">Texte en image</t></si><si><t xml:space="preserve">Du texte présent dans une balise img</t></si><si><t xml:space="preserve">Ne jamais mettre de texte dans une balise img</t></si><si><t xml:space="preserve">Attribut image</t></si><si><t xml:space="preserve">Attribut des images texte mal décrite</t></si><si><t xml:space="preserve">Mettre une description approprié pour l’image porteuse d’information </t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  règle N°113</t></si><si><t xml:space="preserve">Formulaire</t></si><si><t xml:space="preserve">Annuaire -Liste</t></si><si><t xml:space="preserve">Liste annuaire mal construite et spam</t></si><si><t xml:space="preserve">Ne plus faire d’annuaire</t></si><si><t xml:space="preserve">Navigation</t></si><si><t xml:space="preserve">  Les titres h1-h2-h3</t></si><si><t xml:space="preserve"> Titre pas dans l’ordre H3 avant h2</t></si><si><t xml:space="preserve"> Mettre les titres dans l’ordre h1-h2 -h3</t></si><si><t xml:space="preserve">Security</t></si><si><t xml:space="preserve">Liens</t></si><si><t xml:space="preserve">Liens sans libellé</t></si><si><t xml:space="preserve">Liens sans libellé. Qui risque de ne pas être perçu ou incorrectement &#10;compris par les utilisateurs et moteurs de recherche</t></si><si><t xml:space="preserve">Un lien se compose au minimum d’une Url et d’un libellé </t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°131</t></si><si><t xml:space="preserve">Identification et contact</t></si><si><t xml:space="preserve">Données personnalisés</t></si><si><t xml:space="preserve">Serveur et performance</t></si></sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -214,7 +28,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="23">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -334,6 +148,14 @@
       <family val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="12"/>
       <name val=""/>
       <family val="1"/>
@@ -346,6 +168,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -511,7 +340,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -532,14 +361,14 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -548,7 +377,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -560,11 +389,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -572,15 +401,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -679,15 +512,15 @@
   </sheetPr>
   <dimension ref="A1:Z33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="61.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="62.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="58.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="94.72"/>
@@ -967,24 +800,34 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="F17" s="11"/>
+      <c r="A17" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F18" s="13" t="s">
         <v>41</v>
@@ -1010,16 +853,16 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4" t="s">
@@ -1042,7 +885,7 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1055,17 +898,30 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E26" s="16"/>
-      <c r="F26" s="7"/>
+        <v>61</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="16"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1074,7 +930,7 @@
       <c r="F28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="17"/>
+      <c r="A29" s="18"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -1082,18 +938,18 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="17"/>
+      <c r="A31" s="18"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -2077,13 +1933,14 @@
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="F19:F20"/>
-    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="C26:C27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" display="https://checklists.opquast.com/fr/"/>
     <hyperlink ref="F7" r:id="rId2" display="https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html"/>
     <hyperlink ref="F9" r:id="rId3" display="https://www.alsacreations.com/astuce/lire/78-Quelle-est-la-difference-entre-les-chemins-relatifs-et-absolus-.html"/>
     <hyperlink ref="F11" r:id="rId4" display="    http://www.php-astux.info/chemins-relatif-absolu.php"/>
+    <hyperlink ref="F17" r:id="rId5" display="https://checklists.opquast.com/fr/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Validator w3c  et css. Fonctonnement OK. Aucune erreur.
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="UTF-8" standalone="yes"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="69"><si><t xml:space="preserve">Catégorie</t></si><si><t xml:space="preserve">Problème identifié</t></si><si><t xml:space="preserve">Explication du problème</t></si><si><t xml:space="preserve">Bonne pratique à adopter</t></si><si><t xml:space="preserve">Action recommandée</t></si><si><t xml:space="preserve">Référence</t></si><si><t xml:space="preserve">Présentation</t></si><si><t xml:space="preserve">Contraste de la page</t></si><si><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">Problèmes de contraste entre le texte et l’arrière plan</t></r><r><rPr><b val="true"/><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">(accessibilité)</t></r></si><si><t xml:space="preserve">Un ratio de contraste minimal de 3:1 entre le texte et son arrière-plan</t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°177</t></si><si><t xml:space="preserve">Langue page2</t></si><si><t xml:space="preserve">          Langue / défaut </t></si><si><t xml:space="preserve">  Mettre la langue VF</t></si><si><t xml:space="preserve">Cours </t></si><si><t xml:space="preserve">Structure-Code</t></si><si><t xml:space="preserve">Meta</t></si><si><t xml:space="preserve">  Meta /obsolete </t></si><si><t xml:space="preserve">    Enlever la méta keywords</t></si><si><t xml:space="preserve"> Title sans de valeur Page principale et « page 2 » pour la seconde page.</t></si><si><t xml:space="preserve"> Mettre des mots clefs qui correspondent &#10;Au sujet principal du site 70 caractères maximum</t></si><si><t xml:space="preserve">&#10;</t></si><si><t xml:space="preserve">Cours</t></si><si><t xml:space="preserve"> Meta description sans de valeur.</t></si><si><t xml:space="preserve">  Mettre entre  70 -320 caractères </t></si><si><t xml:space="preserve">https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html</t></si><si><t xml:space="preserve"> .  HREF</t></si><si><t xml:space="preserve">   Chemin local pour les valeur Href  </t></si><si><t xml:space="preserve"> Mettre des chemins relatifs </t></si><si><t xml:space="preserve">https://www.alsacreations.com/astuce/lire/78-Quelle-est-la-difference-entre-les-chemins-relatifs-et-absolus-.html</t></si><si><t xml:space="preserve">    http://www.php-astux.info/chemins-relatif-absolu.php</t></si><si><t xml:space="preserve"> CSS balise style</t></si><si><t xml:space="preserve"> Pas de précence d’aria dans les pages</t></si><si><t xml:space="preserve"> Mettre des ARIA pour les personnes handicapés</t></si><si><t xml:space="preserve">  URL </t></si><si><t xml:space="preserve">  URL pas adapté</t></si><si><t xml:space="preserve">  Mettre une adresse URL adapté au sujet</t></si><si><t xml:space="preserve">Image et média</t></si><si><t xml:space="preserve">Répétition ALT  IMG</t></si><si><t xml:space="preserve">  Répétition dans les attributs  des images</t></si><si><t xml:space="preserve"> Mettre des Alt différents (éviter les spams)</t></si><si><t xml:space="preserve"> Cours</t></si><si><t xml:space="preserve">Format d’image</t></si><si><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/></rPr><t xml:space="preserve">Mauvais format d’image bmp  trop lourde +6Mo.</t></r><r><rPr><b val="true"/><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/></rPr><t xml:space="preserve"> ( Vitesse et taille du site )</t></r></si><si><t xml:space="preserve">Format JPEG ou PeG ou GIF</t></si><si><t xml:space="preserve">Texte en image</t></si><si><t xml:space="preserve">Du texte présent dans une balise img</t></si><si><t xml:space="preserve">Ne jamais mettre de texte dans une balise img</t></si><si><t xml:space="preserve">Attribut image</t></si><si><t xml:space="preserve">Attribut des images texte mal décrite</t></si><si><t xml:space="preserve">Mettre une description approprié pour l’image porteuse d’information </t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  règle N°113</t></si><si><t xml:space="preserve">Formulaire</t></si><si><t xml:space="preserve">Annuaire -Liste</t></si><si><t xml:space="preserve">Liste annuaire mal construite et spam</t></si><si><t xml:space="preserve">Ne plus faire d’annuaire</t></si><si><t xml:space="preserve">Navigation</t></si><si><t xml:space="preserve">  Les titres h1-h2-h3</t></si><si><t xml:space="preserve"> Titre pas dans l’ordre H3 avant h2</t></si><si><t xml:space="preserve"> Mettre les titres dans l’ordre h1-h2 -h3</t></si><si><t xml:space="preserve">Security</t></si><si><t xml:space="preserve">Liens</t></si><si><t xml:space="preserve">Liens sans libellé</t></si><si><t xml:space="preserve">Liens sans libellé. Qui risque de ne pas être perçu ou incorrectement &#10;compris par les utilisateurs et moteurs de recherche</t></si><si><t xml:space="preserve">Un lien se compose au minimum d’une Url et d’un libellé </t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°131</t></si><si><t xml:space="preserve">Identification et contact</t></si><si><t xml:space="preserve">Données personnalisés</t></si><si><t xml:space="preserve">Serveur et performance</t></si></sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="72"><si><t xml:space="preserve">Catégorie</t></si><si><t xml:space="preserve">Problème identifié</t></si><si><t xml:space="preserve">Explication du problème</t></si><si><t xml:space="preserve">Bonne pratique à adopter</t></si><si><t xml:space="preserve">Action recommandée</t></si><si><t xml:space="preserve">Référence</t></si><si><t xml:space="preserve">Présentation</t></si><si><t xml:space="preserve">Contraste de la page</t></si><si><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">Problèmes de contraste entre le texte et l’arrière plan</t></r><r><rPr><b val="true"/><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">(accessibilité)</t></r></si><si><t xml:space="preserve">Un ratio de contraste minimal de 3:1 entre le texte et son arrière-plan</t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°177</t></si><si><t xml:space="preserve">Langue page2</t></si><si><t xml:space="preserve">          Langue / défaut </t></si><si><t xml:space="preserve">  Mettre la langue VF</t></si><si><t xml:space="preserve">Cours </t></si><si><t xml:space="preserve">Structure-Code</t></si><si><t xml:space="preserve">Meta</t></si><si><t xml:space="preserve">  Meta /obsolete </t></si><si><t xml:space="preserve">    Enlever la méta keywords</t></si><si><t xml:space="preserve"> Title sans de valeur Page principale et « page 2 » pour la seconde page.</t></si><si><t xml:space="preserve"> Mettre des mots clefs qui correspondent &#10;Au sujet principal du site 70 caractères maximum</t></si><si><t xml:space="preserve">&#10;</t></si><si><t xml:space="preserve">Cours</t></si><si><t xml:space="preserve"> Meta description sans de valeur.</t></si><si><t xml:space="preserve">  Mettre entre  70 -320 caractères </t></si><si><t xml:space="preserve">https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html</t></si><si><t xml:space="preserve"> .  HREF</t></si><si><t xml:space="preserve">   Chemin local pour les valeur Href  </t></si><si><t xml:space="preserve"> Mettre des chemins relatifs </t></si><si><t xml:space="preserve">https://www.alsacreations.com/astuce/lire/78-Quelle-est-la-difference-entre-les-chemins-relatifs-et-absolus-.html</t></si><si><t xml:space="preserve">Logo page 2</t></si><si><t xml:space="preserve">Texte sur une image ( logo page 2)</t></si><si><t xml:space="preserve">Ne jamais mettre de texte sur une image</t></si><si><t xml:space="preserve">    http://www.php-astux.info/chemins-relatif-absolu.php</t></si><si><t xml:space="preserve"> CSS balise style</t></si><si><t xml:space="preserve"> Pas de précence d’aria dans les pages</t></si><si><t xml:space="preserve"> Mettre des ARIA pour les personnes handicapés</t></si><si><t xml:space="preserve">  URL </t></si><si><t xml:space="preserve">  URL pas adapté</t></si><si><t xml:space="preserve">  Mettre une adresse URL adapté au sujet</t></si><si><t xml:space="preserve">Image et média</t></si><si><t xml:space="preserve">Répétition ALT  IMG</t></si><si><t xml:space="preserve">  Répétition dans les attributs  des images</t></si><si><t xml:space="preserve"> Mettre des Alt différents (éviter les spams)</t></si><si><t xml:space="preserve"> Cours</t></si><si><t xml:space="preserve">Format d’image</t></si><si><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/></rPr><t xml:space="preserve">Mauvais format d’image bmp  trop lourde +6Mo.</t></r><r><rPr><b val="true"/><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/></rPr><t xml:space="preserve"> ( Vitesse et taille du site )</t></r></si><si><t xml:space="preserve">Format JPEG ou PeG ou GIF</t></si><si><t xml:space="preserve">Texte en image</t></si><si><t xml:space="preserve">Du texte présent dans une balise img</t></si><si><t xml:space="preserve">Ne jamais mettre de texte dans une balise img</t></si><si><t xml:space="preserve">Attribut image</t></si><si><t xml:space="preserve">Attribut des images texte mal décrite</t></si><si><t xml:space="preserve">Mettre une description approprié pour l’image porteuse d’information </t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  règle N°113</t></si><si><t xml:space="preserve">Formulaire</t></si><si><t xml:space="preserve">Annuaire -Liste</t></si><si><t xml:space="preserve">Liste annuaire mal construite et spam</t></si><si><t xml:space="preserve">Ne plus faire d’annuaire</t></si><si><t xml:space="preserve">Navigation</t></si><si><t xml:space="preserve">  Les titres h1-h2-h3</t></si><si><t xml:space="preserve"> Titre pas dans l’ordre H3 avant h2</t></si><si><t xml:space="preserve"> Mettre les titres dans l’ordre h1-h2 -h3</t></si><si><t xml:space="preserve">Security</t></si><si><t xml:space="preserve">Liens</t></si><si><t xml:space="preserve">Liens sans libellé</t></si><si><t xml:space="preserve">Liens sans libellé. Qui risque de ne pas être perçu ou incorrectement &#10;compris par les utilisateurs et moteurs de recherche</t></si><si><t xml:space="preserve">Un lien se compose au minimum d’une Url et d’un libellé </t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°131-N°132</t></si><si><t xml:space="preserve">Identification et contact</t></si><si><t xml:space="preserve">Données personnalisés</t></si><si><t xml:space="preserve">Serveur et performance</t></si></sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -512,8 +512,8 @@
   </sheetPr>
   <dimension ref="A1:Z33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -693,10 +693,18 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
+      <c r="A10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>32</v>
+      </c>
       <c r="E10" s="12"/>
       <c r="F10" s="10"/>
     </row>
@@ -707,7 +715,7 @@
       <c r="D11" s="11"/>
       <c r="E11" s="12"/>
       <c r="F11" s="11" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -715,13 +723,13 @@
         <v>15</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="11" t="s">
@@ -733,13 +741,13 @@
         <v>15</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="11" t="s">
@@ -748,34 +756,34 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="4" t="s">
@@ -784,16 +792,16 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>22</v>
@@ -801,36 +809,36 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -853,16 +861,16 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4" t="s">
@@ -885,7 +893,7 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -898,20 +906,20 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E26" s="17"/>
       <c r="F26" s="17" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -921,7 +929,7 @@
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -938,7 +946,7 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -949,7 +957,7 @@
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>

</xml_diff>

<commit_message>
6eme recommendation. Capture test.
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="UTF-8" standalone="yes"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="72"><si><t xml:space="preserve">Catégorie</t></si><si><t xml:space="preserve">Problème identifié</t></si><si><t xml:space="preserve">Explication du problème</t></si><si><t xml:space="preserve">Bonne pratique à adopter</t></si><si><t xml:space="preserve">Action recommandée</t></si><si><t xml:space="preserve">Référence</t></si><si><t xml:space="preserve">Présentation</t></si><si><t xml:space="preserve">Contraste de la page</t></si><si><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">Problèmes de contraste entre le texte et l’arrière plan</t></r><r><rPr><b val="true"/><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">(accessibilité)</t></r></si><si><t xml:space="preserve">Un ratio de contraste minimal de 3:1 entre le texte et son arrière-plan</t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°177</t></si><si><t xml:space="preserve">Langue page2</t></si><si><t xml:space="preserve">          Langue / défaut </t></si><si><t xml:space="preserve">  Mettre la langue VF</t></si><si><t xml:space="preserve">Cours </t></si><si><t xml:space="preserve">Structure-Code</t></si><si><t xml:space="preserve">Meta</t></si><si><t xml:space="preserve">  Meta /obsolete </t></si><si><t xml:space="preserve">    Enlever la méta keywords</t></si><si><t xml:space="preserve"> Title sans de valeur Page principale et « page 2 » pour la seconde page.</t></si><si><t xml:space="preserve"> Mettre des mots clefs qui correspondent &#10;Au sujet principal du site 70 caractères maximum</t></si><si><t xml:space="preserve">&#10;</t></si><si><t xml:space="preserve">Cours</t></si><si><t xml:space="preserve"> Meta description sans de valeur.</t></si><si><t xml:space="preserve">  Mettre entre  70 -320 caractères </t></si><si><t xml:space="preserve">https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html</t></si><si><t xml:space="preserve"> .  HREF</t></si><si><t xml:space="preserve">   Chemin local pour les valeur Href  </t></si><si><t xml:space="preserve"> Mettre des chemins relatifs </t></si><si><t xml:space="preserve">https://www.alsacreations.com/astuce/lire/78-Quelle-est-la-difference-entre-les-chemins-relatifs-et-absolus-.html</t></si><si><t xml:space="preserve">Logo page 2</t></si><si><t xml:space="preserve">Texte sur une image ( logo page 2)</t></si><si><t xml:space="preserve">Ne jamais mettre de texte sur une image</t></si><si><t xml:space="preserve">    http://www.php-astux.info/chemins-relatif-absolu.php</t></si><si><t xml:space="preserve"> CSS balise style</t></si><si><t xml:space="preserve"> Pas de précence d’aria dans les pages</t></si><si><t xml:space="preserve"> Mettre des ARIA pour les personnes handicapés</t></si><si><t xml:space="preserve">  URL </t></si><si><t xml:space="preserve">  URL pas adapté</t></si><si><t xml:space="preserve">  Mettre une adresse URL adapté au sujet</t></si><si><t xml:space="preserve">Image et média</t></si><si><t xml:space="preserve">Répétition ALT  IMG</t></si><si><t xml:space="preserve">  Répétition dans les attributs  des images</t></si><si><t xml:space="preserve"> Mettre des Alt différents (éviter les spams)</t></si><si><t xml:space="preserve"> Cours</t></si><si><t xml:space="preserve">Format d’image</t></si><si><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/></rPr><t xml:space="preserve">Mauvais format d’image bmp  trop lourde +6Mo.</t></r><r><rPr><b val="true"/><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/></rPr><t xml:space="preserve"> ( Vitesse et taille du site )</t></r></si><si><t xml:space="preserve">Format JPEG ou PeG ou GIF</t></si><si><t xml:space="preserve">Texte en image</t></si><si><t xml:space="preserve">Du texte présent dans une balise img</t></si><si><t xml:space="preserve">Ne jamais mettre de texte dans une balise img</t></si><si><t xml:space="preserve">Attribut image</t></si><si><t xml:space="preserve">Attribut des images texte mal décrite</t></si><si><t xml:space="preserve">Mettre une description approprié pour l’image porteuse d’information </t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  règle N°113</t></si><si><t xml:space="preserve">Formulaire</t></si><si><t xml:space="preserve">Annuaire -Liste</t></si><si><t xml:space="preserve">Liste annuaire mal construite et spam</t></si><si><t xml:space="preserve">Ne plus faire d’annuaire</t></si><si><t xml:space="preserve">Navigation</t></si><si><t xml:space="preserve">  Les titres h1-h2-h3</t></si><si><t xml:space="preserve"> Titre pas dans l’ordre H3 avant h2</t></si><si><t xml:space="preserve"> Mettre les titres dans l’ordre h1-h2 -h3</t></si><si><t xml:space="preserve">Security</t></si><si><t xml:space="preserve">Liens</t></si><si><t xml:space="preserve">Liens sans libellé</t></si><si><t xml:space="preserve">Liens sans libellé. Qui risque de ne pas être perçu ou incorrectement &#10;compris par les utilisateurs et moteurs de recherche</t></si><si><t xml:space="preserve">Un lien se compose au minimum d’une Url et d’un libellé </t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°131-N°132</t></si><si><t xml:space="preserve">Identification et contact</t></si><si><t xml:space="preserve">Données personnalisés</t></si><si><t xml:space="preserve">Serveur et performance</t></si></sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="72"><si><t xml:space="preserve">Catégorie</t></si><si><t xml:space="preserve">Problème identifié</t></si><si><t xml:space="preserve">Explication du problème</t></si><si><t xml:space="preserve">Bonne pratique à adopter</t></si><si><t xml:space="preserve">Action recommandée</t></si><si><t xml:space="preserve">Référence</t></si><si><t xml:space="preserve">Présentation</t></si><si><t xml:space="preserve">Contraste de la page</t></si><si><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">Problèmes de contraste entre le texte et l’arrière plan</t></r><r><rPr><b val="true"/><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">(accessibilité)</t></r></si><si><t xml:space="preserve">Un ratio de contraste minimal de 3:1 entre le texte et son arrière-plan</t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°177</t></si><si><t xml:space="preserve">Langue page2</t></si><si><t xml:space="preserve">          Langue / défaut </t></si><si><t xml:space="preserve">  Mettre la langue VF</t></si><si><t xml:space="preserve">Cours </t></si><si><t xml:space="preserve">Structure-Code</t></si><si><t xml:space="preserve">Meta</t></si><si><t xml:space="preserve">  Meta /obsolete </t></si><si><t xml:space="preserve">    Enlever la méta keywords</t></si><si><t xml:space="preserve"> Title sans de valeur Page principale et « page 2 » pour la seconde page.</t></si><si><t xml:space="preserve"> Mettre des mots clefs qui correspondent &#10;Au sujet principal du site 70 caractères maximum</t></si><si><t xml:space="preserve">&#10;</t></si><si><t xml:space="preserve">Cours</t></si><si><t xml:space="preserve"> Meta description sans de valeur.</t></si><si><t xml:space="preserve">  Mettre entre  70 -320 caractères </t></si><si><t xml:space="preserve">https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html</t></si><si><t xml:space="preserve"> .  HREF</t></si><si><t xml:space="preserve">   Chemin local pour les valeur Href  </t></si><si><t xml:space="preserve"> Mettre des chemins relatifs </t></si><si><t xml:space="preserve">https://www.alsacreations.com/astuce/lire/78-Quelle-est-la-difference-entre-les-chemins-relatifs-et-absolus-.html</t></si><si><t xml:space="preserve">Logo page 2</t></si><si><t xml:space="preserve">Texte sur une image ( logo page 2)</t></si><si><t xml:space="preserve">Ne jamais mettre de texte sur une image</t></si><si><t xml:space="preserve">  URL </t></si><si><t xml:space="preserve">  URL pas adapté</t></si><si><t xml:space="preserve">  Mettre une adresse URL adapté au sujet</t></si><si><t xml:space="preserve">    http://www.php-astux.info/chemins-relatif-absolu.php</t></si><si><t xml:space="preserve"> CSS balise style</t></si><si><t xml:space="preserve"> Pas de précence d’aria dans les pages</t></si><si><t xml:space="preserve"> Mettre des ARIA pour les personnes handicapés</t></si><si><t xml:space="preserve">Navigation</t></si><si><t xml:space="preserve">  Les titres h1-h2-h3</t></si><si><t xml:space="preserve"> Titre pas dans l’ordre H3 avant h2</t></si><si><t xml:space="preserve"> Mettre les titres dans l’ordre h1-h2 -h3</t></si><si><t xml:space="preserve">Image et média</t></si><si><t xml:space="preserve">Répétition ALT  IMG</t></si><si><t xml:space="preserve">  Répétition dans les attributs  des images</t></si><si><t xml:space="preserve"> Mettre des Alt différents (éviter les spams)</t></si><si><t xml:space="preserve"> Cours</t></si><si><t xml:space="preserve">Format d’image</t></si><si><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/></rPr><t xml:space="preserve">Mauvais format d’image bmp  trop lourde +6Mo.</t></r><r><rPr><b val="true"/><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/></rPr><t xml:space="preserve"> ( Vitesse et taille du site )</t></r></si><si><t xml:space="preserve">Format JPEG ou PeG ou GIF</t></si><si><t xml:space="preserve">Texte en image</t></si><si><t xml:space="preserve">Du texte présent dans une balise img</t></si><si><t xml:space="preserve">Ne jamais mettre de texte dans une balise img</t></si><si><t xml:space="preserve">Attribut image</t></si><si><t xml:space="preserve">Attribut des images texte mal décrite</t></si><si><t xml:space="preserve">Mettre une description approprié pour l’image porteuse d’information </t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  règle N°113</t></si><si><t xml:space="preserve">Formulaire</t></si><si><t xml:space="preserve">Annuaire -Liste</t></si><si><t xml:space="preserve">Liste annuaire mal construite et spam</t></si><si><t xml:space="preserve">Ne plus faire d’annuaire</t></si><si><t xml:space="preserve">Liens</t></si><si><t xml:space="preserve">Liens sans libellé</t></si><si><t xml:space="preserve">Liens sans libellé. Qui risque de ne pas être perçu ou incorrectement &#10;compris par les utilisateurs et moteurs de recherche</t></si><si><t xml:space="preserve">Un lien se compose au minimum d’une Url et d’un libellé </t></si><si><t xml:space="preserve">Security</t></si><si><t xml:space="preserve">Identification et contact</t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°131-N°132</t></si><si><t xml:space="preserve">Données personnalisés</t></si><si><t xml:space="preserve">Serveur et performance</t></si></sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -401,12 +401,12 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -510,10 +510,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z33"/>
+  <dimension ref="A1:Z31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -709,13 +709,21 @@
       <c r="F10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
+      <c r="A11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>35</v>
+      </c>
       <c r="E11" s="12"/>
       <c r="F11" s="11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -723,13 +731,13 @@
         <v>15</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="11" t="s">
@@ -737,17 +745,17 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>39</v>
+      <c r="A13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>43</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="11" t="s">
@@ -756,34 +764,34 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="4" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="4" t="s">
@@ -792,16 +800,16 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>22</v>
@@ -809,36 +817,36 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -852,26 +860,26 @@
       <c r="F19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
+      <c r="A20" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>66</v>
+      </c>
       <c r="E20" s="14"/>
       <c r="F20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>62</v>
-      </c>
+      <c r="A21" s="3"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="13"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4" t="s">
         <v>22</v>
@@ -879,9 +887,9 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="5"/>
@@ -893,7 +901,7 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -906,30 +914,24 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C26" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>67</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="B26" s="11"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="11"/>
       <c r="E26" s="17"/>
       <c r="F26" s="17" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="11"/>
       <c r="B27" s="11"/>
-      <c r="C27" s="16"/>
+      <c r="C27" s="11"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -946,23 +948,14 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="18"/>
-    </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-    </row>
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1941,7 +1934,7 @@
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="F19:F20"/>
-    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C20:C21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" display="https://checklists.opquast.com/fr/"/>

</xml_diff>

<commit_message>
7eme Changement. Security. Mise en place de la securité de codage : Integrity Sha256-Filehash pour les données extérieures scripts.
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="UTF-8" standalone="yes"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="72"><si><t xml:space="preserve">Catégorie</t></si><si><t xml:space="preserve">Problème identifié</t></si><si><t xml:space="preserve">Explication du problème</t></si><si><t xml:space="preserve">Bonne pratique à adopter</t></si><si><t xml:space="preserve">Action recommandée</t></si><si><t xml:space="preserve">Référence</t></si><si><t xml:space="preserve">Présentation</t></si><si><t xml:space="preserve">Contraste de la page</t></si><si><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">Problèmes de contraste entre le texte et l’arrière plan</t></r><r><rPr><b val="true"/><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">(accessibilité)</t></r></si><si><t xml:space="preserve">Un ratio de contraste minimal de 3:1 entre le texte et son arrière-plan</t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°177</t></si><si><t xml:space="preserve">Langue page2</t></si><si><t xml:space="preserve">          Langue / défaut </t></si><si><t xml:space="preserve">  Mettre la langue VF</t></si><si><t xml:space="preserve">Cours </t></si><si><t xml:space="preserve">Structure-Code</t></si><si><t xml:space="preserve">Meta</t></si><si><t xml:space="preserve">  Meta /obsolete </t></si><si><t xml:space="preserve">    Enlever la méta keywords</t></si><si><t xml:space="preserve"> Title sans de valeur Page principale et « page 2 » pour la seconde page.</t></si><si><t xml:space="preserve"> Mettre des mots clefs qui correspondent &#10;Au sujet principal du site 70 caractères maximum</t></si><si><t xml:space="preserve">&#10;</t></si><si><t xml:space="preserve">Cours</t></si><si><t xml:space="preserve"> Meta description sans de valeur.</t></si><si><t xml:space="preserve">  Mettre entre  70 -320 caractères </t></si><si><t xml:space="preserve">https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html</t></si><si><t xml:space="preserve"> .  HREF</t></si><si><t xml:space="preserve">   Chemin local pour les valeur Href  </t></si><si><t xml:space="preserve"> Mettre des chemins relatifs </t></si><si><t xml:space="preserve">https://www.alsacreations.com/astuce/lire/78-Quelle-est-la-difference-entre-les-chemins-relatifs-et-absolus-.html</t></si><si><t xml:space="preserve">Logo page 2</t></si><si><t xml:space="preserve">Texte sur une image ( logo page 2)</t></si><si><t xml:space="preserve">Ne jamais mettre de texte sur une image</t></si><si><t xml:space="preserve">  URL </t></si><si><t xml:space="preserve">  URL pas adapté</t></si><si><t xml:space="preserve">  Mettre une adresse URL adapté au sujet</t></si><si><t xml:space="preserve">    http://www.php-astux.info/chemins-relatif-absolu.php</t></si><si><t xml:space="preserve"> CSS balise style</t></si><si><t xml:space="preserve"> Pas de précence d’aria dans les pages</t></si><si><t xml:space="preserve"> Mettre des ARIA pour les personnes handicapés</t></si><si><t xml:space="preserve">Navigation</t></si><si><t xml:space="preserve">  Les titres h1-h2-h3</t></si><si><t xml:space="preserve"> Titre pas dans l’ordre H3 avant h2</t></si><si><t xml:space="preserve"> Mettre les titres dans l’ordre h1-h2 -h3</t></si><si><t xml:space="preserve">Image et média</t></si><si><t xml:space="preserve">Répétition ALT  IMG</t></si><si><t xml:space="preserve">  Répétition dans les attributs  des images</t></si><si><t xml:space="preserve"> Mettre des Alt différents (éviter les spams)</t></si><si><t xml:space="preserve"> Cours</t></si><si><t xml:space="preserve">Format d’image</t></si><si><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/></rPr><t xml:space="preserve">Mauvais format d’image bmp  trop lourde +6Mo.</t></r><r><rPr><b val="true"/><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/></rPr><t xml:space="preserve"> ( Vitesse et taille du site )</t></r></si><si><t xml:space="preserve">Format JPEG ou PeG ou GIF</t></si><si><t xml:space="preserve">Texte en image</t></si><si><t xml:space="preserve">Du texte présent dans une balise img</t></si><si><t xml:space="preserve">Ne jamais mettre de texte dans une balise img</t></si><si><t xml:space="preserve">Attribut image</t></si><si><t xml:space="preserve">Attribut des images texte mal décrite</t></si><si><t xml:space="preserve">Mettre une description approprié pour l’image porteuse d’information </t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  règle N°113</t></si><si><t xml:space="preserve">Formulaire</t></si><si><t xml:space="preserve">Annuaire -Liste</t></si><si><t xml:space="preserve">Liste annuaire mal construite et spam</t></si><si><t xml:space="preserve">Ne plus faire d’annuaire</t></si><si><t xml:space="preserve">Liens</t></si><si><t xml:space="preserve">Liens sans libellé</t></si><si><t xml:space="preserve">Liens sans libellé. Qui risque de ne pas être perçu ou incorrectement &#10;compris par les utilisateurs et moteurs de recherche</t></si><si><t xml:space="preserve">Un lien se compose au minimum d’une Url et d’un libellé </t></si><si><t xml:space="preserve">Security</t></si><si><t xml:space="preserve">Identification et contact</t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°131-N°132</t></si><si><t xml:space="preserve">Données personnalisés</t></si><si><t xml:space="preserve">Serveur et performance</t></si></sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="73"><si><t xml:space="preserve">Catégorie</t></si><si><t xml:space="preserve">Problème identifié</t></si><si><t xml:space="preserve">Explication du problème</t></si><si><t xml:space="preserve">Bonne pratique à adopter</t></si><si><t xml:space="preserve">Action recommandée</t></si><si><t xml:space="preserve">Référence</t></si><si><t xml:space="preserve">Présentation</t></si><si><t xml:space="preserve">Contraste de la page</t></si><si><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">Problèmes de contraste entre le texte et l’arrière plan</t></r><r><rPr><b val="true"/><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">(accessibilité)</t></r></si><si><t xml:space="preserve">Un ratio de contraste minimal de 3:1 entre le texte et son arrière-plan</t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°177</t></si><si><t xml:space="preserve">Langue page2</t></si><si><t xml:space="preserve">          Langue / défaut </t></si><si><t xml:space="preserve">  Mettre la langue VF</t></si><si><t xml:space="preserve">Cours </t></si><si><t xml:space="preserve">Structure-Code</t></si><si><t xml:space="preserve">Meta</t></si><si><t xml:space="preserve">  Meta /obsolete </t></si><si><t xml:space="preserve">    Enlever la méta keywords</t></si><si><t xml:space="preserve"> Title sans de valeur Page principale et « page 2 » pour la seconde page.</t></si><si><t xml:space="preserve"> Mettre des mots clefs qui correspondent &#10;Au sujet principal du site 70 caractères maximum</t></si><si><t xml:space="preserve">&#10;</t></si><si><t xml:space="preserve">Cours</t></si><si><t xml:space="preserve"> Meta description sans de valeur.</t></si><si><t xml:space="preserve">  Mettre entre  70 -320 caractères </t></si><si><t xml:space="preserve">https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html</t></si><si><t xml:space="preserve"> .  HREF</t></si><si><t xml:space="preserve">   Chemin local pour les valeur Href  </t></si><si><t xml:space="preserve"> Mettre des chemins relatifs </t></si><si><t xml:space="preserve">https://www.alsacreations.com/astuce/lire/78-Quelle-est-la-difference-entre-les-chemins-relatifs-et-absolus-.html</t></si><si><t xml:space="preserve">Logo page 2</t></si><si><t xml:space="preserve">Texte sur une image ( logo page 2)</t></si><si><t xml:space="preserve">Ne jamais mettre de texte sur une image</t></si><si><t xml:space="preserve">  URL </t></si><si><t xml:space="preserve">  URL pas adapté</t></si><si><t xml:space="preserve">  Mettre une adresse URL adapté au sujet</t></si><si><t xml:space="preserve">    http://www.php-astux.info/chemins-relatif-absolu.php</t></si><si><t xml:space="preserve"> CSS balise style</t></si><si><t xml:space="preserve"> Pas de précence d’aria dans les pages</t></si><si><t xml:space="preserve"> Mettre des ARIA pour les personnes handicapés</t></si><si><t xml:space="preserve">Navigation</t></si><si><t xml:space="preserve">  Les titres h1-h2-h3</t></si><si><t xml:space="preserve"> Titre pas dans l’ordre H3 avant h2</t></si><si><t xml:space="preserve"> Mettre les titres dans l’ordre h1-h2 -h3</t></si><si><t xml:space="preserve">Image et média</t></si><si><t xml:space="preserve">Répétition ALT  IMG</t></si><si><t xml:space="preserve">  Répétition dans les attributs  des images</t></si><si><t xml:space="preserve"> Mettre des Alt différents (éviter les spams)</t></si><si><t xml:space="preserve"> Cours</t></si><si><t xml:space="preserve">Format d’image</t></si><si><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/></rPr><t xml:space="preserve">Mauvais format d’image bmp  trop lourde +6Mo.</t></r><r><rPr><b val="true"/><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/></rPr><t xml:space="preserve"> ( Vitesse et taille du site )</t></r></si><si><t xml:space="preserve">Format JPEG ou PeG ou GIF</t></si><si><t xml:space="preserve">Texte en image</t></si><si><t xml:space="preserve">Du texte présent dans une balise img</t></si><si><t xml:space="preserve">Ne jamais mettre de texte dans une balise img</t></si><si><t xml:space="preserve">Attribut image</t></si><si><t xml:space="preserve">Attribut des images texte mal décrite</t></si><si><t xml:space="preserve">Mettre une description approprié pour l’image porteuse d’information </t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  règle N°113</t></si><si><t xml:space="preserve">Formulaire</t></si><si><t xml:space="preserve">Annuaire -Liste</t></si><si><t xml:space="preserve">Liste annuaire mal construite et spam</t></si><si><t xml:space="preserve">Ne plus faire d’annuaire</t></si><si><t xml:space="preserve">Liens</t></si><si><t xml:space="preserve">Liens sans libellé</t></si><si><t xml:space="preserve">Liens sans libellé. Qui risque de ne pas être perçu ou incorrectement &#10;compris par les utilisateurs et moteurs de recherche</t></si><si><t xml:space="preserve">Un lien se compose au minimum d’une Url et d’un libellé </t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°131-N°132</t></si><si><t xml:space="preserve">Security</t></si><si><t xml:space="preserve">https://www.w3schools.com/tags/att_script_integrity.asp ou https://checklists.opquast.com/fr/  règle n° 209</t></si><si><t xml:space="preserve">Identification et contact</t></si><si><t xml:space="preserve">Données personnalisés</t></si><si><t xml:space="preserve">Serveur et performance</t></si></sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -340,7 +340,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -403,6 +403,10 @@
     </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -512,8 +516,8 @@
   </sheetPr>
   <dimension ref="A1:Z31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -873,7 +877,9 @@
         <v>66</v>
       </c>
       <c r="E20" s="14"/>
-      <c r="F20" s="10"/>
+      <c r="F20" s="16" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="3"/>
@@ -887,9 +893,9 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="5"/>
@@ -901,7 +907,10 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -914,15 +923,13 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="13"/>
       <c r="D26" s="11"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17" t="s">
-        <v>69</v>
-      </c>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="11"/>
@@ -931,7 +938,7 @@
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -940,7 +947,7 @@
       <c r="F28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="18"/>
+      <c r="A29" s="19"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -948,7 +955,7 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1925,15 +1932,13 @@
     <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="7">
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="F9:F10"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
     <mergeCell ref="C20:C21"/>
   </mergeCells>
   <hyperlinks>

</xml_diff>

<commit_message>
8eme Recommandation. Identification et contact Nouveau title et nom pour chaque page. Page Index est remplacé par "La Chouette Agence Design à Lyon." Page 2 est remplacé par   "Formulaire-de-Contact " Modification de la taille du  logo page 2 également.
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="UTF-8" standalone="yes"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="73"><si><t xml:space="preserve">Catégorie</t></si><si><t xml:space="preserve">Problème identifié</t></si><si><t xml:space="preserve">Explication du problème</t></si><si><t xml:space="preserve">Bonne pratique à adopter</t></si><si><t xml:space="preserve">Action recommandée</t></si><si><t xml:space="preserve">Référence</t></si><si><t xml:space="preserve">Présentation</t></si><si><t xml:space="preserve">Contraste de la page</t></si><si><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">Problèmes de contraste entre le texte et l’arrière plan</t></r><r><rPr><b val="true"/><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">(accessibilité)</t></r></si><si><t xml:space="preserve">Un ratio de contraste minimal de 3:1 entre le texte et son arrière-plan</t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°177</t></si><si><t xml:space="preserve">Langue page2</t></si><si><t xml:space="preserve">          Langue / défaut </t></si><si><t xml:space="preserve">  Mettre la langue VF</t></si><si><t xml:space="preserve">Cours </t></si><si><t xml:space="preserve">Structure-Code</t></si><si><t xml:space="preserve">Meta</t></si><si><t xml:space="preserve">  Meta /obsolete </t></si><si><t xml:space="preserve">    Enlever la méta keywords</t></si><si><t xml:space="preserve"> Title sans de valeur Page principale et « page 2 » pour la seconde page.</t></si><si><t xml:space="preserve"> Mettre des mots clefs qui correspondent &#10;Au sujet principal du site 70 caractères maximum</t></si><si><t xml:space="preserve">&#10;</t></si><si><t xml:space="preserve">Cours</t></si><si><t xml:space="preserve"> Meta description sans de valeur.</t></si><si><t xml:space="preserve">  Mettre entre  70 -320 caractères </t></si><si><t xml:space="preserve">https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html</t></si><si><t xml:space="preserve"> .  HREF</t></si><si><t xml:space="preserve">   Chemin local pour les valeur Href  </t></si><si><t xml:space="preserve"> Mettre des chemins relatifs </t></si><si><t xml:space="preserve">https://www.alsacreations.com/astuce/lire/78-Quelle-est-la-difference-entre-les-chemins-relatifs-et-absolus-.html</t></si><si><t xml:space="preserve">Logo page 2</t></si><si><t xml:space="preserve">Texte sur une image ( logo page 2)</t></si><si><t xml:space="preserve">Ne jamais mettre de texte sur une image</t></si><si><t xml:space="preserve">  URL </t></si><si><t xml:space="preserve">  URL pas adapté</t></si><si><t xml:space="preserve">  Mettre une adresse URL adapté au sujet</t></si><si><t xml:space="preserve">    http://www.php-astux.info/chemins-relatif-absolu.php</t></si><si><t xml:space="preserve"> CSS balise style</t></si><si><t xml:space="preserve"> Pas de précence d’aria dans les pages</t></si><si><t xml:space="preserve"> Mettre des ARIA pour les personnes handicapés</t></si><si><t xml:space="preserve">Navigation</t></si><si><t xml:space="preserve">  Les titres h1-h2-h3</t></si><si><t xml:space="preserve"> Titre pas dans l’ordre H3 avant h2</t></si><si><t xml:space="preserve"> Mettre les titres dans l’ordre h1-h2 -h3</t></si><si><t xml:space="preserve">Image et média</t></si><si><t xml:space="preserve">Répétition ALT  IMG</t></si><si><t xml:space="preserve">  Répétition dans les attributs  des images</t></si><si><t xml:space="preserve"> Mettre des Alt différents (éviter les spams)</t></si><si><t xml:space="preserve"> Cours</t></si><si><t xml:space="preserve">Format d’image</t></si><si><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/></rPr><t xml:space="preserve">Mauvais format d’image bmp  trop lourde +6Mo.</t></r><r><rPr><b val="true"/><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/></rPr><t xml:space="preserve"> ( Vitesse et taille du site )</t></r></si><si><t xml:space="preserve">Format JPEG ou PeG ou GIF</t></si><si><t xml:space="preserve">Texte en image</t></si><si><t xml:space="preserve">Du texte présent dans une balise img</t></si><si><t xml:space="preserve">Ne jamais mettre de texte dans une balise img</t></si><si><t xml:space="preserve">Attribut image</t></si><si><t xml:space="preserve">Attribut des images texte mal décrite</t></si><si><t xml:space="preserve">Mettre une description approprié pour l’image porteuse d’information </t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  règle N°113</t></si><si><t xml:space="preserve">Formulaire</t></si><si><t xml:space="preserve">Annuaire -Liste</t></si><si><t xml:space="preserve">Liste annuaire mal construite et spam</t></si><si><t xml:space="preserve">Ne plus faire d’annuaire</t></si><si><t xml:space="preserve">Liens</t></si><si><t xml:space="preserve">Liens sans libellé</t></si><si><t xml:space="preserve">Liens sans libellé. Qui risque de ne pas être perçu ou incorrectement &#10;compris par les utilisateurs et moteurs de recherche</t></si><si><t xml:space="preserve">Un lien se compose au minimum d’une Url et d’un libellé </t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°131-N°132</t></si><si><t xml:space="preserve">Security</t></si><si><t xml:space="preserve">https://www.w3schools.com/tags/att_script_integrity.asp ou https://checklists.opquast.com/fr/  règle n° 209</t></si><si><t xml:space="preserve">Identification et contact</t></si><si><t xml:space="preserve">Données personnalisés</t></si><si><t xml:space="preserve">Serveur et performance</t></si></sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="81"><si><t xml:space="preserve">Catégorie</t></si><si><t xml:space="preserve">Problème identifié</t></si><si><t xml:space="preserve">Explication du problème</t></si><si><t xml:space="preserve">Bonne pratique à adopter</t></si><si><t xml:space="preserve">Action recommandée</t></si><si><t xml:space="preserve">Référence</t></si><si><t xml:space="preserve">Présentation</t></si><si><t xml:space="preserve">Contraste de la page</t></si><si><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">Problèmes de contraste entre le texte et l’arrière plan</t></r><r><rPr><b val="true"/><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">(accessibilité)</t></r></si><si><t xml:space="preserve">Un ratio de contraste minimal de 3:1 entre le texte et son arrière-plan</t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°177</t></si><si><t xml:space="preserve">Langue page2</t></si><si><t xml:space="preserve">          Langue / défaut </t></si><si><t xml:space="preserve">  Mettre la langue VF</t></si><si><t xml:space="preserve">Cours </t></si><si><t xml:space="preserve">Structure-Code</t></si><si><t xml:space="preserve">Meta</t></si><si><t xml:space="preserve">  Meta obsolète </t></si><si><t xml:space="preserve">    Enlever la méta keywords</t></si><si><t xml:space="preserve">Pas d’attribut defer dans les balises Scripts</t></si><si><t xml:space="preserve"> Mettre en différé le chargement des scripts pour charger d’abord le Html et le Css sans bloquer le rendu HTML (son affichage à l&apos;écran)</t></si><si><t xml:space="preserve">&#10;</t></si><si><t xml:space="preserve">https://www.alsacreations.com/astuce/lire/1562-script-attribut-async-defer.html</t></si><si><t xml:space="preserve"> Meta description sans de valeur.</t></si><si><t xml:space="preserve">  Mettre entre  70 -320 caractères </t></si><si><t xml:space="preserve">https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html</t></si><si><t xml:space="preserve"> .  HREF</t></si><si><t xml:space="preserve">   Chemin local pour les valeur Href  balise Link</t></si><si><t xml:space="preserve"> Mettre des chemins relatifs </t></si><si><t xml:space="preserve">https://www.alsacreations.com/astuce/lire/78-Quelle-est-la-difference-entre-les-chemins-relatifs-et-absolus-.html</t></si><si><t xml:space="preserve">Logo page 2</t></si><si><t xml:space="preserve">Texte sur une image ( logo page 2)</t></si><si><t xml:space="preserve">Ne jamais mettre de texte sur une image</t></si><si><t xml:space="preserve">  URL </t></si><si><t xml:space="preserve">  URL pas adapté</t></si><si><t xml:space="preserve">  Mettre une adresse URL adapté au sujet</t></si><si><t xml:space="preserve">    http://www.php-astux.info/chemins-relatif-absolu.php</t></si><si><t xml:space="preserve"> CSS balise style</t></si><si><t xml:space="preserve"> Pas de précence d’aria dans les pages</t></si><si><t xml:space="preserve"> Mettre des ARIA pour les personnes handicapés</t></si><si><t xml:space="preserve">Cours</t></si><si><t xml:space="preserve">Navigation</t></si><si><t xml:space="preserve">  Les titres h1-h2-h3</t></si><si><t xml:space="preserve"> Titre pas dans l’ordre H3 avant h2</t></si><si><t xml:space="preserve"> Mettre les titres dans l’ordre h1-h2 -h3</t></si><si><t xml:space="preserve">Image et média</t></si><si><t xml:space="preserve">Répétition ALT  IMG</t></si><si><t xml:space="preserve">  Répétition dans les attributs  des images</t></si><si><t xml:space="preserve"> Mettre des Alt différents (éviter les spams)</t></si><si><t xml:space="preserve"> Cours</t></si><si><t xml:space="preserve">Format d’image</t></si><si><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/></rPr><t xml:space="preserve">Mauvais format d’image bmp  trop lourde +6Mo.</t></r><r><rPr><b val="true"/><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/></rPr><t xml:space="preserve"> ( Vitesse et taille du site )</t></r></si><si><t xml:space="preserve">Format JPEG ou PeG ou GIF</t></si><si><t xml:space="preserve">Texte en image</t></si><si><t xml:space="preserve">Du texte présent dans une balise img</t></si><si><t xml:space="preserve">Ne jamais mettre de texte dans une balise img</t></si><si><t xml:space="preserve">Attribut image</t></si><si><t xml:space="preserve">Attribut des images texte mal décrite</t></si><si><t xml:space="preserve">Mettre une description approprié pour l’image porteuse d’information </t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  règle N°113</t></si><si><t xml:space="preserve">Formulaire</t></si><si><t xml:space="preserve">Annuaire -Liste</t></si><si><t xml:space="preserve">Liste annuaire mal construite et spam</t></si><si><t xml:space="preserve">Ne plus faire d’annuaire</t></si><si><t xml:space="preserve">Liens</t></si><si><t xml:space="preserve">Liens sans libellé</t></si><si><t xml:space="preserve">Liens sans libellé. Qui risque de ne pas être perçu ou incorrectement &#10;compris par les utilisateurs et moteurs de recherche</t></si><si><t xml:space="preserve">Un lien se compose au minimum d’une Url et d’un libellé </t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°131-N°132</t></si><si><t xml:space="preserve">Security</t></si><si><t xml:space="preserve">Problème de sécurité</t></si><si><t xml:space="preserve">Risques associés à la diffusion de code malveillant désindexation, plaintes&#10;Prévenir les risques de diffusion de code malveillant. </t></si><si><t xml:space="preserve">Vérification que les ressources tierces (fichiers scripts, feuilles de style&#10;…) n’ont pas été modifiées pour y insérer du code malveillant.</t></si><si><t xml:space="preserve">https://www.w3schools.com/tags/att_script_integrity.asp ou https://checklists.opquast.com/fr/  règle n° 209</t></si><si><t xml:space="preserve">Identification et contact</t></si><si><t xml:space="preserve">Title</t></si><si><t xml:space="preserve"> Page principale : Title sans de valeur « . » &#10;Page 2 « page 2 » pour la seconde page.</t></si><si><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">Rédiger le contenu de l&apos;élément title de chaque page&#10;Le titre de chaque page permet d’identifier  </t></r><r><rPr><b val="true"/><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">le nom du site</t></r><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">.</t></r></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°97</t></si><si><t xml:space="preserve">Données personnelles</t></si><si><t xml:space="preserve">Serveur et performance</t></si></sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -340,7 +340,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -361,6 +361,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -381,10 +385,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -397,6 +397,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -406,7 +410,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -415,6 +419,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -516,18 +528,18 @@
   </sheetPr>
   <dimension ref="A1:Z31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="62.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="58.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="64.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="59.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="94.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="123.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="10.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="11.28"/>
   </cols>
@@ -585,12 +597,12 @@
       <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -602,8 +614,8 @@
       <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="4" t="s">
+      <c r="E3" s="7"/>
+      <c r="F3" s="5" t="s">
         <v>14</v>
       </c>
     </row>
@@ -620,40 +632,40 @@
       <c r="D4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4"/>
       <c r="B6" s="11"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="10"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -666,7 +678,7 @@
         <v>24</v>
       </c>
       <c r="E7" s="12"/>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="8" t="s">
         <v>25</v>
       </c>
     </row>
@@ -675,11 +687,11 @@
       <c r="B8" s="11"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -691,13 +703,13 @@
       <c r="D9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="10" t="s">
+      <c r="E9" s="7"/>
+      <c r="F9" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="13" t="s">
@@ -710,10 +722,10 @@
         <v>32</v>
       </c>
       <c r="E10" s="12"/>
-      <c r="F10" s="10"/>
+      <c r="F10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="13" t="s">
@@ -726,12 +738,12 @@
         <v>35</v>
       </c>
       <c r="E11" s="12"/>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="13" t="s">
@@ -744,113 +756,113 @@
         <v>39</v>
       </c>
       <c r="E12" s="12"/>
-      <c r="F12" s="11" t="s">
-        <v>22</v>
+      <c r="F12" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="11" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="B15" s="13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E15" s="12"/>
-      <c r="F15" s="4" t="s">
-        <v>22</v>
+      <c r="F15" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
-        <v>44</v>
+      <c r="A16" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>22</v>
+        <v>55</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
-        <v>44</v>
+      <c r="A17" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="F17" s="13" t="s">
         <v>58</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>48</v>
+        <v>63</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -858,87 +870,105 @@
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
-      <c r="E19" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F19" s="10"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="8"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" s="15" t="s">
         <v>65</v>
       </c>
+      <c r="C20" s="16" t="s">
+        <v>66</v>
+      </c>
       <c r="D20" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" s="14"/>
-      <c r="F20" s="16" t="s">
         <v>67</v>
+      </c>
+      <c r="E20" s="15"/>
+      <c r="F20" s="17" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="3"/>
       <c r="B21" s="13"/>
-      <c r="C21" s="15"/>
+      <c r="C21" s="16"/>
       <c r="D21" s="13"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="4" t="s">
-        <v>22</v>
+      <c r="F21" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="F22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5"/>
+      <c r="A23" s="6"/>
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
       <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
+      <c r="F23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F24" s="0" t="s">
         <v>69</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="11"/>
       <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="7"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="8"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
+        <v>74</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" s="19"/>
+      <c r="F26" s="21" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="11"/>
       <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="21"/>
+      <c r="F27" s="21"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -947,7 +977,7 @@
       <c r="F28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="19"/>
+      <c r="A29" s="22"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -955,7 +985,7 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1932,7 +1962,7 @@
     <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="12">
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
@@ -1940,13 +1970,20 @@
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="F26:F27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" display="https://checklists.opquast.com/fr/"/>
-    <hyperlink ref="F7" r:id="rId2" display="https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html"/>
-    <hyperlink ref="F9" r:id="rId3" display="https://www.alsacreations.com/astuce/lire/78-Quelle-est-la-difference-entre-les-chemins-relatifs-et-absolus-.html"/>
-    <hyperlink ref="F11" r:id="rId4" display="    http://www.php-astux.info/chemins-relatif-absolu.php"/>
-    <hyperlink ref="F17" r:id="rId5" display="https://checklists.opquast.com/fr/"/>
+    <hyperlink ref="F5" r:id="rId2" display="https://www.alsacreations.com/astuce/lire/1562-script-attribut-async-defer.html"/>
+    <hyperlink ref="F7" r:id="rId3" display="https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html"/>
+    <hyperlink ref="F9" r:id="rId4" display="https://www.alsacreations.com/astuce/lire/78-Quelle-est-la-difference-entre-les-chemins-relatifs-et-absolus-.html"/>
+    <hyperlink ref="F11" r:id="rId5" display="    http://www.php-astux.info/chemins-relatif-absolu.php"/>
+    <hyperlink ref="F17" r:id="rId6" display="https://checklists.opquast.com/fr/"/>
+    <hyperlink ref="F26" r:id="rId7" display="https://checklists.opquast.com/fr/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
10eme changement. Serveurs et performance. La racine du site contient des instructions pour les robots d'indexation.
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="UTF-8" standalone="yes"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="81"><si><t xml:space="preserve">Catégorie</t></si><si><t xml:space="preserve">Problème identifié</t></si><si><t xml:space="preserve">Explication du problème</t></si><si><t xml:space="preserve">Bonne pratique à adopter</t></si><si><t xml:space="preserve">Action recommandée</t></si><si><t xml:space="preserve">Référence</t></si><si><t xml:space="preserve">Présentation</t></si><si><t xml:space="preserve">Contraste de la page</t></si><si><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">Problèmes de contraste entre le texte et l’arrière plan</t></r><r><rPr><b val="true"/><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">(accessibilité)</t></r></si><si><t xml:space="preserve">Un ratio de contraste minimal de 3:1 entre le texte et son arrière-plan</t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°177</t></si><si><t xml:space="preserve">Langue page2</t></si><si><t xml:space="preserve">          Langue / défaut </t></si><si><t xml:space="preserve">  Mettre la langue VF</t></si><si><t xml:space="preserve">Cours </t></si><si><t xml:space="preserve">Structure-Code</t></si><si><t xml:space="preserve">Meta</t></si><si><t xml:space="preserve">  Meta obsolète </t></si><si><t xml:space="preserve">    Enlever la méta keywords</t></si><si><t xml:space="preserve">Pas d’attribut defer dans les balises Scripts</t></si><si><t xml:space="preserve"> Mettre en différé le chargement des scripts pour charger d’abord le Html et le Css sans bloquer le rendu HTML (son affichage à l&apos;écran)</t></si><si><t xml:space="preserve">&#10;</t></si><si><t xml:space="preserve">https://www.alsacreations.com/astuce/lire/1562-script-attribut-async-defer.html</t></si><si><t xml:space="preserve"> Meta description sans de valeur.</t></si><si><t xml:space="preserve">  Mettre entre  70 -320 caractères </t></si><si><t xml:space="preserve">https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html</t></si><si><t xml:space="preserve"> .  HREF</t></si><si><t xml:space="preserve">   Chemin local pour les valeur Href  balise Link</t></si><si><t xml:space="preserve"> Mettre des chemins relatifs </t></si><si><t xml:space="preserve">https://www.alsacreations.com/astuce/lire/78-Quelle-est-la-difference-entre-les-chemins-relatifs-et-absolus-.html</t></si><si><t xml:space="preserve">Logo page 2</t></si><si><t xml:space="preserve">Texte sur une image ( logo page 2)</t></si><si><t xml:space="preserve">Ne jamais mettre de texte sur une image</t></si><si><t xml:space="preserve">  URL </t></si><si><t xml:space="preserve">  URL pas adapté</t></si><si><t xml:space="preserve">  Mettre une adresse URL adapté au sujet</t></si><si><t xml:space="preserve">    http://www.php-astux.info/chemins-relatif-absolu.php</t></si><si><t xml:space="preserve"> CSS balise style</t></si><si><t xml:space="preserve"> Pas de précence d’aria dans les pages</t></si><si><t xml:space="preserve"> Mettre des ARIA pour les personnes handicapés</t></si><si><t xml:space="preserve">Cours</t></si><si><t xml:space="preserve">Navigation</t></si><si><t xml:space="preserve">  Les titres h1-h2-h3</t></si><si><t xml:space="preserve"> Titre pas dans l’ordre H3 avant h2</t></si><si><t xml:space="preserve"> Mettre les titres dans l’ordre h1-h2 -h3</t></si><si><t xml:space="preserve">Image et média</t></si><si><t xml:space="preserve">Répétition ALT  IMG</t></si><si><t xml:space="preserve">  Répétition dans les attributs  des images</t></si><si><t xml:space="preserve"> Mettre des Alt différents (éviter les spams)</t></si><si><t xml:space="preserve"> Cours</t></si><si><t xml:space="preserve">Format d’image</t></si><si><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/></rPr><t xml:space="preserve">Mauvais format d’image bmp  trop lourde +6Mo.</t></r><r><rPr><b val="true"/><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/></rPr><t xml:space="preserve"> ( Vitesse et taille du site )</t></r></si><si><t xml:space="preserve">Format JPEG ou PeG ou GIF</t></si><si><t xml:space="preserve">Texte en image</t></si><si><t xml:space="preserve">Du texte présent dans une balise img</t></si><si><t xml:space="preserve">Ne jamais mettre de texte dans une balise img</t></si><si><t xml:space="preserve">Attribut image</t></si><si><t xml:space="preserve">Attribut des images texte mal décrite</t></si><si><t xml:space="preserve">Mettre une description approprié pour l’image porteuse d’information </t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  règle N°113</t></si><si><t xml:space="preserve">Formulaire</t></si><si><t xml:space="preserve">Annuaire -Liste</t></si><si><t xml:space="preserve">Liste annuaire mal construite et spam</t></si><si><t xml:space="preserve">Ne plus faire d’annuaire</t></si><si><t xml:space="preserve">Liens</t></si><si><t xml:space="preserve">Liens sans libellé</t></si><si><t xml:space="preserve">Liens sans libellé. Qui risque de ne pas être perçu ou incorrectement &#10;compris par les utilisateurs et moteurs de recherche</t></si><si><t xml:space="preserve">Un lien se compose au minimum d’une Url et d’un libellé </t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°131-N°132</t></si><si><t xml:space="preserve">Security</t></si><si><t xml:space="preserve">Problème de sécurité</t></si><si><t xml:space="preserve">Risques associés à la diffusion de code malveillant désindexation, plaintes&#10;Prévenir les risques de diffusion de code malveillant. </t></si><si><t xml:space="preserve">Vérification que les ressources tierces (fichiers scripts, feuilles de style&#10;…) n’ont pas été modifiées pour y insérer du code malveillant.</t></si><si><t xml:space="preserve">https://www.w3schools.com/tags/att_script_integrity.asp ou https://checklists.opquast.com/fr/  règle n° 209</t></si><si><t xml:space="preserve">Identification et contact</t></si><si><t xml:space="preserve">Title</t></si><si><t xml:space="preserve"> Page principale : Title sans de valeur « . » &#10;Page 2 « page 2 » pour la seconde page.</t></si><si><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">Rédiger le contenu de l&apos;élément title de chaque page&#10;Le titre de chaque page permet d’identifier  </t></r><r><rPr><b val="true"/><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">le nom du site</t></r><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">.</t></r></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°97</t></si><si><t xml:space="preserve">Données personnelles</t></si><si><t xml:space="preserve">Serveur et performance</t></si></sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="99"><si><t xml:space="preserve">Catégorie</t></si><si><t xml:space="preserve">Problème identifié</t></si><si><t xml:space="preserve">Explication du problème</t></si><si><t xml:space="preserve">Bonne pratique à adopter</t></si><si><t xml:space="preserve">Action recommandée</t></si><si><t xml:space="preserve">Référence</t></si><si><r><rPr><sz val="12"/><color rgb="FF007FFF"/><rFont val=""/><family val="1"/></rPr><t xml:space="preserve">Présentation(</t></r><r><rPr><b val="true"/><sz val="12"/><color rgb="FF007FFF"/><rFont val=""/><family val="1"/></rPr><t xml:space="preserve">accessibilité)</t></r></si><si><t xml:space="preserve">Contraste de la page</t></si><si><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">Problèmes de contraste entre le texte et l’arrière plan</t></r><r><rPr><b val="true"/><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">(accessibilité)</t></r></si><si><t xml:space="preserve">Un ratio de contraste minimal de 3:1 entre le texte et son arrière-plan</t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°177</t></si><si><t xml:space="preserve">Présentation</t></si><si><t xml:space="preserve">Langue page2</t></si><si><t xml:space="preserve">          Langue / défaut </t></si><si><t xml:space="preserve">  Mettre la langue VF</t></si><si><t xml:space="preserve">Cours</t></si><si><t xml:space="preserve">Présentation-Accessibilité</t></si><si><t xml:space="preserve">Valeur justify utiliser</t></si><si><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">Ne pas utiliser la propriété CSS text-align avec la valeur </t></r><r><rPr><b val="true"/><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">justify</t></r><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">, ou tout autre équivalent.</t></r></si><si><t xml:space="preserve">Les styles ne justifient pas le texte.</t></si><si><t xml:space="preserve"> https://checklists.opquast.com/fr/ Règle N°186</t></si><si><t xml:space="preserve">Structure-Code</t></si><si><t xml:space="preserve">Meta</t></si><si><t xml:space="preserve">  Meta obsolète </t></si><si><t xml:space="preserve">    Enlever la méta keywords</t></si><si><t xml:space="preserve">Cours </t></si><si><t xml:space="preserve">Pas d’attribut defer dans les balises Scripts&#10;Les pages mettent donc plus de temps à charger</t></si><si><t xml:space="preserve"> Mettre en différé le chargement des scripts pour charger d’abord le Html et le Css sans bloquer le rendu HTML (son affichage à l&apos;écran)</t></si><si><t xml:space="preserve">&#10;</t></si><si><t xml:space="preserve">https://www.alsacreations.com/astuce/lire/1562-script-attribut-async-defer.html</t></si><si><t xml:space="preserve">https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html</t></si><si><t xml:space="preserve"> CSS balise style</t></si><si><t xml:space="preserve"> Pas de précence d’aria dans les pages</t></si><si><t xml:space="preserve"> Mettre des ARIA pour les personnes handicapés</t></si><si><t xml:space="preserve"> .  HREF</t></si><si><t xml:space="preserve">   Chemin local pour les valeur Href  balise Link</t></si><si><t xml:space="preserve"> Mettre des chemins relatifs </t></si><si><t xml:space="preserve">https://www.alsacreations.com/astuce/lire/78-Quelle-est-la-difference-entre-les-chemins-relatifs-et-absolus-.html</t></si><si><t xml:space="preserve">Logo page 2</t></si><si><t xml:space="preserve">Texte sur une image ( logo page 2)</t></si><si><t xml:space="preserve">Ne jamais mettre de texte sur une image</t></si><si><t xml:space="preserve">  URL </t></si><si><t xml:space="preserve">  URL pas adapté</t></si><si><t xml:space="preserve">  Mettre une adresse URL adapté au sujet</t></si><si><t xml:space="preserve">    http://www.php-astux.info/chemins-relatif-absolu.php</t></si><si><t xml:space="preserve">Contenus</t></si><si><t xml:space="preserve"> Meta description sans de valeur.</t></si><si><t xml:space="preserve">Renseigner la balise &lt;meta name=&quot;description&quot; content=&quot;&quot; /&gt;</t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°3</t></si><si><t xml:space="preserve">Navigation</t></si><si><t xml:space="preserve">  Les titres h1-h2-h3</t></si><si><t xml:space="preserve"> Titre pas dans l’ordre H3 avant h2</t></si><si><t xml:space="preserve"> Mettre les titres dans l’ordre h1-h2 -h3</t></si><si><t xml:space="preserve">Image et média</t></si><si><t xml:space="preserve">Répétition ALT  IMG</t></si><si><t xml:space="preserve">  Répétition dans les attributs  des images</t></si><si><t xml:space="preserve"> Mettre des Alt différents (éviter les spams)</t></si><si><t xml:space="preserve"> Cours</t></si><si><t xml:space="preserve">Image et média(Vitesse-taille du site)</t></si><si><t xml:space="preserve">Format d’image</t></si><si><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/></rPr><t xml:space="preserve">Mauvais format d’image bmp  trop lourde +6Mo.</t></r><r><rPr><b val="true"/><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/></rPr><t xml:space="preserve"> ( Vitesse et taille du site )</t></r></si><si><t xml:space="preserve">Format JPEG ou PeG ou GIF</t></si><si><t xml:space="preserve">Texte en image</t></si><si><t xml:space="preserve">Du texte présent dans une balise img</t></si><si><t xml:space="preserve">Ne jamais mettre de texte dans une balise img</t></si><si><t xml:space="preserve">Attribut image</t></si><si><t xml:space="preserve">Attribut des images texte mal décrite</t></si><si><t xml:space="preserve">Mettre une description approprié pour l’image porteuse d’information </t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  règle N°113</t></si><si><t xml:space="preserve">Formulaire</t></si><si><t xml:space="preserve">Annuaire -Liste</t></si><si><t xml:space="preserve">Liste annuaire mal construite et spam</t></si><si><t xml:space="preserve">Ne plus faire d’annuaire</t></si><si><t xml:space="preserve">Liens</t></si><si><t xml:space="preserve">Liens sans libellé</t></si><si><t xml:space="preserve">Liens sans libellé. Qui risque de ne pas être perçu ou incorrectement &#10;compris par les utilisateurs et moteurs de recherche</t></si><si><t xml:space="preserve">Un lien se compose au minimum d’une Url et d’un libellé </t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°131-N°132</t></si><si><t xml:space="preserve">Security</t></si><si><t xml:space="preserve">Problème de sécurité</t></si><si><t xml:space="preserve">Risques associés à la diffusion de code malveillant désindexation, plaintes&#10;Prévenir les risques de diffusion de code malveillant. </t></si><si><t xml:space="preserve">Vérification que les ressources tierces (fichiers scripts, feuilles de style&#10;…) n’ont pas été modifiées pour y insérer du code malveillant.</t></si><si><t xml:space="preserve">https://www.w3schools.com/tags/att_script_integrity.asp ou https://checklists.opquast.com/fr/  règle n° 209</t></si><si><t xml:space="preserve">Identification et contact</t></si><si><t xml:space="preserve">Title</t></si><si><t xml:space="preserve"> Page principale : Title sans de valeur « . » &#10;Page 2 « page 2 » pour la seconde page.</t></si><si><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">Rédiger le contenu de l&apos;élément title de chaque page&#10;Le titre de chaque page permet d’identifier  </t></r><r><rPr><b val="true"/><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">le nom du site</t></r><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">.</t></r></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°97</t></si><si><t xml:space="preserve">Serveur et performance</t></si><si><t xml:space="preserve">Problème d&apos;indexation</t></si><si><t xml:space="preserve">Diminuer l&apos;impact énergétique lié à la consultation du site. </t></si><si><t xml:space="preserve">Alternativement, pour agir au niveau d&apos;une page spécifique, utiliser dans celle-ci&#10; La balise meta name=&quot;robots&quot; content=&quot;attribut1, attribut2&quot; : </t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°212</t></si><si><t xml:space="preserve">Recommendations supplémentaire</t></si><si><t xml:space="preserve">Performance</t></si><si><t xml:space="preserve">Le site propose un fichier sitemap indiquant les contenus à explorer</t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°213</t></si><si><t xml:space="preserve">Minimiser la quantité de données à télécharger par l&apos;utilisateur. </t></si><si><t xml:space="preserve">Supprimer les espaces non nécessaires et les commentaires dans les fichiers &#10;CSS en recourant à des outils dédiés.</t></si></sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -28,7 +28,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="26">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -150,6 +150,13 @@
     <font>
       <b val="true"/>
       <sz val="12"/>
+      <color rgb="FF007FFF"/>
+      <name val=""/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
@@ -182,9 +189,22 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val=""/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val=""/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="10">
@@ -215,7 +235,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
+        <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
     <fill>
@@ -340,7 +360,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -365,55 +385,59 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -421,7 +445,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -429,7 +453,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -462,13 +494,13 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF996600"/>
@@ -526,19 +558,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z31"/>
+  <dimension ref="A1:Z35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="64.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="59.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="74.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="69.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="123.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="10.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="11.28"/>
@@ -603,398 +635,460 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>15</v>
+      <c r="A4" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>14</v>
+        <v>19</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
-        <v>15</v>
+      <c r="A5" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="B6" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="8"/>
+      <c r="C6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="8" t="s">
-        <v>25</v>
-      </c>
+      <c r="A7" s="4"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="8"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="12" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>28</v>
+        <v>21</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>33</v>
       </c>
       <c r="E9" s="7"/>
-      <c r="F9" s="8" t="s">
-        <v>29</v>
-      </c>
+      <c r="F9" s="12"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="8"/>
+        <v>21</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="12" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="5" t="s">
-        <v>36</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="12"/>
+        <v>21</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="14"/>
       <c r="F12" s="5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>43</v>
+        <v>45</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="5" t="s">
-        <v>40</v>
+        <v>47</v>
+      </c>
+      <c r="E13" s="14"/>
+      <c r="F13" s="8" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="5" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="E15" s="12"/>
+      <c r="A15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="7"/>
       <c r="F15" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>55</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="14"/>
       <c r="F16" s="5" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F19" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="D17" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="8"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="17" t="s">
-        <v>68</v>
-      </c>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="12"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="F22" s="5"/>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="16"/>
+      <c r="F21" s="18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="4"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
       <c r="F23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>73</v>
-      </c>
+      <c r="A24" s="6"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="11"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="8"/>
+      <c r="A25" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C26" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D26" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="E26" s="19"/>
-      <c r="F26" s="21" t="s">
-        <v>78</v>
-      </c>
+      <c r="A26" s="13"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="12"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="11"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="21"/>
-      <c r="F27" s="21"/>
+      <c r="A27" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="E27" s="20"/>
+      <c r="F27" s="22" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="22"/>
+      <c r="F28" s="22"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="22"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
+      <c r="A29" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" s="22" t="s">
+        <v>91</v>
+      </c>
       <c r="E29" s="4"/>
+      <c r="F29" s="4" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="A30" s="24"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="15"/>
+    </row>
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="F31" s="19"/>
+    </row>
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="25"/>
+      <c r="F32" s="8"/>
+    </row>
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>92</v>
+      </c>
+    </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1961,29 +2055,33 @@
     <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1001" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="F26:F27"/>
+  <mergeCells count="14">
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="D34:D35"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" display="https://checklists.opquast.com/fr/"/>
-    <hyperlink ref="F5" r:id="rId2" display="https://www.alsacreations.com/astuce/lire/1562-script-attribut-async-defer.html"/>
-    <hyperlink ref="F7" r:id="rId3" display="https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html"/>
-    <hyperlink ref="F9" r:id="rId4" display="https://www.alsacreations.com/astuce/lire/78-Quelle-est-la-difference-entre-les-chemins-relatifs-et-absolus-.html"/>
-    <hyperlink ref="F11" r:id="rId5" display="    http://www.php-astux.info/chemins-relatif-absolu.php"/>
-    <hyperlink ref="F17" r:id="rId6" display="https://checklists.opquast.com/fr/"/>
-    <hyperlink ref="F26" r:id="rId7" display="https://checklists.opquast.com/fr/"/>
+    <hyperlink ref="F4" r:id="rId2" display="https://checklists.opquast.com/fr/"/>
+    <hyperlink ref="F6" r:id="rId3" display="https://www.alsacreations.com/astuce/lire/1562-script-attribut-async-defer.html"/>
+    <hyperlink ref="F8" r:id="rId4" display="https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html"/>
+    <hyperlink ref="F10" r:id="rId5" display="https://www.alsacreations.com/astuce/lire/78-Quelle-est-la-difference-entre-les-chemins-relatifs-et-absolus-.html"/>
+    <hyperlink ref="F12" r:id="rId6" display="    http://www.php-astux.info/chemins-relatif-absolu.php"/>
+    <hyperlink ref="F18" r:id="rId7" display="https://checklists.opquast.com/fr/"/>
+    <hyperlink ref="F27" r:id="rId8" display="https://checklists.opquast.com/fr/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Modification contraste colour texte formulaire. Page Formulaire-de-contact.
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -560,8 +560,8 @@
   </sheetPr>
   <dimension ref="A1:Z35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Ajout du fichier audit. Suite au bug d'enregistrement ...
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="UTF-8" standalone="yes"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="99"><si><t xml:space="preserve">Catégorie</t></si><si><t xml:space="preserve">Problème identifié</t></si><si><t xml:space="preserve">Explication du problème</t></si><si><t xml:space="preserve">Bonne pratique à adopter</t></si><si><t xml:space="preserve">Action recommandée</t></si><si><t xml:space="preserve">Référence</t></si><si><r><rPr><sz val="12"/><color rgb="FF007FFF"/><rFont val=""/><family val="1"/></rPr><t xml:space="preserve">Présentation(</t></r><r><rPr><b val="true"/><sz val="12"/><color rgb="FF007FFF"/><rFont val=""/><family val="1"/></rPr><t xml:space="preserve">accessibilité)</t></r></si><si><t xml:space="preserve">Contraste de la page</t></si><si><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">Problèmes de contraste entre le texte et l’arrière plan</t></r><r><rPr><b val="true"/><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">(accessibilité)</t></r></si><si><t xml:space="preserve">Un ratio de contraste minimal de 3:1 entre le texte et son arrière-plan</t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°177</t></si><si><t xml:space="preserve">Présentation</t></si><si><t xml:space="preserve">Langue page2</t></si><si><t xml:space="preserve">          Langue / défaut </t></si><si><t xml:space="preserve">  Mettre la langue VF</t></si><si><t xml:space="preserve">Cours</t></si><si><t xml:space="preserve">Présentation-Accessibilité</t></si><si><t xml:space="preserve">Valeur justify utiliser</t></si><si><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">Ne pas utiliser la propriété CSS text-align avec la valeur </t></r><r><rPr><b val="true"/><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">justify</t></r><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">, ou tout autre équivalent.</t></r></si><si><t xml:space="preserve">Les styles ne justifient pas le texte.</t></si><si><t xml:space="preserve"> https://checklists.opquast.com/fr/ Règle N°186</t></si><si><t xml:space="preserve">Structure-Code</t></si><si><t xml:space="preserve">Meta</t></si><si><t xml:space="preserve">  Meta obsolète </t></si><si><t xml:space="preserve">    Enlever la méta keywords</t></si><si><t xml:space="preserve">Cours </t></si><si><t xml:space="preserve">Pas d’attribut defer dans les balises Scripts&#10;Les pages mettent donc plus de temps à charger</t></si><si><t xml:space="preserve"> Mettre en différé le chargement des scripts pour charger d’abord le Html et le Css sans bloquer le rendu HTML (son affichage à l&apos;écran)</t></si><si><t xml:space="preserve">&#10;</t></si><si><t xml:space="preserve">https://www.alsacreations.com/astuce/lire/1562-script-attribut-async-defer.html</t></si><si><t xml:space="preserve">https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html</t></si><si><t xml:space="preserve"> CSS balise style</t></si><si><t xml:space="preserve"> Pas de précence d’aria dans les pages</t></si><si><t xml:space="preserve"> Mettre des ARIA pour les personnes handicapés</t></si><si><t xml:space="preserve"> .  HREF</t></si><si><t xml:space="preserve">   Chemin local pour les valeur Href  balise Link</t></si><si><t xml:space="preserve"> Mettre des chemins relatifs </t></si><si><t xml:space="preserve">https://www.alsacreations.com/astuce/lire/78-Quelle-est-la-difference-entre-les-chemins-relatifs-et-absolus-.html</t></si><si><t xml:space="preserve">Logo page 2</t></si><si><t xml:space="preserve">Texte sur une image ( logo page 2)</t></si><si><t xml:space="preserve">Ne jamais mettre de texte sur une image</t></si><si><t xml:space="preserve">  URL </t></si><si><t xml:space="preserve">  URL pas adapté</t></si><si><t xml:space="preserve">  Mettre une adresse URL adapté au sujet</t></si><si><t xml:space="preserve">    http://www.php-astux.info/chemins-relatif-absolu.php</t></si><si><t xml:space="preserve">Contenus</t></si><si><t xml:space="preserve"> Meta description sans de valeur.</t></si><si><t xml:space="preserve">Renseigner la balise &lt;meta name=&quot;description&quot; content=&quot;&quot; /&gt;</t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°3</t></si><si><t xml:space="preserve">Navigation</t></si><si><t xml:space="preserve">  Les titres h1-h2-h3</t></si><si><t xml:space="preserve"> Titre pas dans l’ordre H3 avant h2</t></si><si><t xml:space="preserve"> Mettre les titres dans l’ordre h1-h2 -h3</t></si><si><t xml:space="preserve">Image et média</t></si><si><t xml:space="preserve">Répétition ALT  IMG</t></si><si><t xml:space="preserve">  Répétition dans les attributs  des images</t></si><si><t xml:space="preserve"> Mettre des Alt différents (éviter les spams)</t></si><si><t xml:space="preserve"> Cours</t></si><si><t xml:space="preserve">Image et média(Vitesse-taille du site)</t></si><si><t xml:space="preserve">Format d’image</t></si><si><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/></rPr><t xml:space="preserve">Mauvais format d’image bmp  trop lourde +6Mo.</t></r><r><rPr><b val="true"/><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/></rPr><t xml:space="preserve"> ( Vitesse et taille du site )</t></r></si><si><t xml:space="preserve">Format JPEG ou PeG ou GIF</t></si><si><t xml:space="preserve">Texte en image</t></si><si><t xml:space="preserve">Du texte présent dans une balise img</t></si><si><t xml:space="preserve">Ne jamais mettre de texte dans une balise img</t></si><si><t xml:space="preserve">Attribut image</t></si><si><t xml:space="preserve">Attribut des images texte mal décrite</t></si><si><t xml:space="preserve">Mettre une description approprié pour l’image porteuse d’information </t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  règle N°113</t></si><si><t xml:space="preserve">Formulaire</t></si><si><t xml:space="preserve">Annuaire -Liste</t></si><si><t xml:space="preserve">Liste annuaire mal construite et spam</t></si><si><t xml:space="preserve">Ne plus faire d’annuaire</t></si><si><t xml:space="preserve">Liens</t></si><si><t xml:space="preserve">Liens sans libellé</t></si><si><t xml:space="preserve">Liens sans libellé. Qui risque de ne pas être perçu ou incorrectement &#10;compris par les utilisateurs et moteurs de recherche</t></si><si><t xml:space="preserve">Un lien se compose au minimum d’une Url et d’un libellé </t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°131-N°132</t></si><si><t xml:space="preserve">Security</t></si><si><t xml:space="preserve">Problème de sécurité</t></si><si><t xml:space="preserve">Risques associés à la diffusion de code malveillant désindexation, plaintes&#10;Prévenir les risques de diffusion de code malveillant. </t></si><si><t xml:space="preserve">Vérification que les ressources tierces (fichiers scripts, feuilles de style&#10;…) n’ont pas été modifiées pour y insérer du code malveillant.</t></si><si><t xml:space="preserve">https://www.w3schools.com/tags/att_script_integrity.asp ou https://checklists.opquast.com/fr/  règle n° 209</t></si><si><t xml:space="preserve">Identification et contact</t></si><si><t xml:space="preserve">Title</t></si><si><t xml:space="preserve"> Page principale : Title sans de valeur « . » &#10;Page 2 « page 2 » pour la seconde page.</t></si><si><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">Rédiger le contenu de l&apos;élément title de chaque page&#10;Le titre de chaque page permet d’identifier  </t></r><r><rPr><b val="true"/><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">le nom du site</t></r><r><rPr><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">.</t></r></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°97</t></si><si><t xml:space="preserve">Serveur et performance</t></si><si><t xml:space="preserve">Problème d&apos;indexation</t></si><si><t xml:space="preserve">Diminuer l&apos;impact énergétique lié à la consultation du site. </t></si><si><t xml:space="preserve">Alternativement, pour agir au niveau d&apos;une page spécifique, utiliser dans celle-ci&#10; La balise meta name=&quot;robots&quot; content=&quot;attribut1, attribut2&quot; : </t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°212</t></si><si><t xml:space="preserve">Recommendations supplémentaire</t></si><si><t xml:space="preserve">Performance</t></si><si><t xml:space="preserve">Le site propose un fichier sitemap indiquant les contenus à explorer</t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°213</t></si><si><t xml:space="preserve">Minimiser la quantité de données à télécharger par l&apos;utilisateur. </t></si><si><t xml:space="preserve">Supprimer les espaces non nécessaires et les commentaires dans les fichiers &#10;CSS en recourant à des outils dédiés.</t></si></sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="89"><si><t xml:space="preserve">Catégorie</t></si><si><t xml:space="preserve">Problème identifié</t></si><si><t xml:space="preserve">Explication du problème</t></si><si><t xml:space="preserve">Bonne pratique à adopter</t></si><si><t xml:space="preserve">Action recommandée</t></si><si><t xml:space="preserve">Référence</t></si><si><r><rPr><sz val="12"/><color rgb="FF007FFF"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">Présentation</t></r><r><rPr><b val="true"/><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">(Accessibilité)</t></r></si><si><t xml:space="preserve">Contraste de la page</t></si><si><r><rPr><sz val="11"/><rFont val="Calibri"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">Problèmes de contraste entre le texte et l’arrière plan</t></r><r><rPr><b val="true"/><sz val="11"/><rFont val="Calibri"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">(accessibilité)</t></r></si><si><t xml:space="preserve">Un ratio de contraste minimal de 3:1 entre le texte et son arrière-plan</t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/  Règle N°177</t></si><si><t xml:space="preserve">Présentation</t></si><si><t xml:space="preserve">Langue page2</t></si><si><t xml:space="preserve">          Langue / défaut </t></si><si><t xml:space="preserve">  Mettre la langue VF</t></si><si><t xml:space="preserve">Cours </t></si><si><t xml:space="preserve">Structure-Code</t></si><si><t xml:space="preserve">Meta</t></si><si><t xml:space="preserve">  Meta /obsolete </t></si><si><t xml:space="preserve">    Enlever la méta keywords</t></si><si><t xml:space="preserve"> Title sans de valeur Page principale et « page 2 » pour la seconde page.</t></si><si><t xml:space="preserve"> Mettre des mots clefs qui correspondent &#10;Au sujet principal du site 70 caractères maximum</t></si><si><t xml:space="preserve">&#10;</t></si><si><t xml:space="preserve">Cours</t></si><si><t xml:space="preserve"> Meta description sans de valeur.</t></si><si><t xml:space="preserve">  Mettre entre  70 -320 caractères </t></si><si><t xml:space="preserve">https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html</t></si><si><t xml:space="preserve"> .  HREF</t></si><si><t xml:space="preserve">   Chemin local pour les valeur Href  </t></si><si><t xml:space="preserve"> Mettre des chemins relatifs </t></si><si><t xml:space="preserve">https://www.alsacreations.com/astuce/lire/78-Quelle-est-la-difference-entre-les-chemins-relatifs-et-absolus-.html</t></si><si><t xml:space="preserve">Logo page 2</t></si><si><t xml:space="preserve">Texte sur une image ( logo page 2)</t></si><si><t xml:space="preserve">Ne jamais mettre de texte sur une image</t></si><si><t xml:space="preserve">  URL </t></si><si><t xml:space="preserve">  URL pas adapté</t></si><si><t xml:space="preserve">  Mettre une adresse URL adapté au sujet</t></si><si><t xml:space="preserve">    http://www.php-astux.info/chemins-relatif-absolu.php</t></si><si><t xml:space="preserve"> CSS balise style</t></si><si><t xml:space="preserve"> Pas de précence d’aria dans les pages</t></si><si><t xml:space="preserve"> Mettre des ARIA pour les personnes handicapés</t></si><si><t xml:space="preserve">Navigation</t></si><si><t xml:space="preserve">  Les titres h1-h2-h3</t></si><si><t xml:space="preserve"> Titre pas dans l’ordre H3 avant h2</t></si><si><t xml:space="preserve"> Mettre les titres dans l’ordre h1-h2 -h3</t></si><si><t xml:space="preserve">Image et média</t></si><si><t xml:space="preserve">Répétition ALT  IMG</t></si><si><t xml:space="preserve">  Répétition dans les attributs  des images</t></si><si><t xml:space="preserve">Chaque image porteuse d&apos;information est dotée d&apos;une alternative textuelle appropriée</t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/   Règle N°°113</t></si><si><r><rPr><sz val="12"/><rFont val="Arial"/><family val="0"/></rPr><t xml:space="preserve">Image et média&#10;</t></r><r><rPr><b val="true"/><sz val="12"/><color rgb="FF000000"/><rFont val="Arial"/><family val="0"/></rPr><t xml:space="preserve">(Vitesse et taille du site)</t></r></si><si><t xml:space="preserve">Format d’image</t></si><si><r><rPr><sz val="11"/><rFont val="Calibri"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve">Mauvais format d’image bmp  trop lourde +6Mo.</t></r><r><rPr><b val="true"/><sz val="11"/><rFont val="Calibri"/><family val="0"/><charset val="1"/></rPr><t xml:space="preserve"> ( Vitesse et taille du site )</t></r></si><si><t xml:space="preserve">Format JPEG ou PeG ou GIF</t></si><si><t xml:space="preserve">Texte en image</t></si><si><t xml:space="preserve">Du texte présent dans une balise img</t></si><si><t xml:space="preserve">Ne jamais mettre de texte dans une balise img</t></si><si><t xml:space="preserve">Attribut image</t></si><si><t xml:space="preserve">Attribut des images texte mal décrite</t></si><si><t xml:space="preserve">Mettre une description approprié pour l’image porteuse d’information </t></si><si><t xml:space="preserve">Formulaire</t></si><si><t xml:space="preserve">Accessibilité</t></si><si><t xml:space="preserve">Problème de compréhension pour les personnes handicapés </t></si><si><t xml:space="preserve">Chaque champ de formulaire est associé dans le code source à une étiquette qui lui est propre</t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/   Règle N°°67</t></si><si><t xml:space="preserve">Security</t></si><si><t xml:space="preserve">Manque de sécurité</t></si><si><t xml:space="preserve">Prévenir les risques de diffusion de code malveillant. </t></si><si><t xml:space="preserve">Utiliser l&apos;attribut integrity de chaque élément link et script (appelant un fichier externe) </t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/   Règle N°209 ou&#10; https://developer.mozilla.org/fr/docs/Web/HTML/Element/script&#10;</t></si><si><t xml:space="preserve">Liens</t></si><si><t xml:space="preserve">Améliorer l’accessibilité des contenus aux personnes handicapées</t></si><si><t xml:space="preserve">Un lien se compose au minimum d’une Url et d’un libellé</t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/   Règle N°131</t></si><si><t xml:space="preserve">Données Personnelles </t></si><si><t xml:space="preserve">Serveur et performance</t></si><si><t xml:space="preserve">Contenus</t></si><si><t xml:space="preserve">Recommandations&#10;Supplémentaires</t></si><si><t xml:space="preserve">On ne laisse pas à l&apos;utilisateur le contrôle des animations lors de la consultation du contenu. </t></si><si><t xml:space="preserve">Les animations, sons et clignotements peuvent être mis en pause, en muet  ou être arrêté </t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/   Règle N°121</t></si><si><t xml:space="preserve">Accessibilité&#10;Développement</t></si><si><t xml:space="preserve">Optimiser le rendu dans les lecteurs d’écran en permettant d’expliciter les étiquettes des &#10;Champs de formulaire.Améliorer l’accessibilité des contenus aux personnes handicapées</t></si><si><t xml:space="preserve">Les informations complétant l&apos;étiquette d&apos;un champ sont associées &#10;À celui-ci dans le code-source&#10;</t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/   Règle N°68</t></si><si><t xml:space="preserve">Certificat </t></si><si><t xml:space="preserve">   S’assurer que les certificats  sont signés et en cours de validité </t></si><si><t xml:space="preserve">Permettre aux utilisateurs de connaître la validité du certificat et contribuer&#10;à la sécurisation de la transaction.</t></si><si><t xml:space="preserve">https://checklists.opquast.com/fr/   Règle N°193</t></si></sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -144,15 +144,9 @@
     <font>
       <sz val="12"/>
       <color rgb="FF007FFF"/>
-      <name val=""/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FF007FFF"/>
-      <name val=""/>
-      <family val="1"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -163,9 +157,23 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="12"/>
-      <name val=""/>
-      <family val="1"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -181,6 +189,11 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -189,22 +202,9 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val=""/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val=""/>
-      <family val="1"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="10">
@@ -360,7 +360,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -381,11 +381,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -394,7 +390,15 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -402,67 +406,55 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -558,20 +550,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z35"/>
+  <dimension ref="A1:Z65536"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="74.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="69.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="123.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="77.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="80.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="94.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="10.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="11.28"/>
   </cols>
@@ -623,13 +615,13 @@
       <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -647,12 +639,12 @@
         <v>14</v>
       </c>
       <c r="E3" s="7"/>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -664,440 +656,461 @@
       <c r="D4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="D5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="E5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="F5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="4" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="11"/>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="D7" s="12" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="9" t="s">
+      <c r="E7" s="13"/>
+      <c r="F7" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="12"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="12" t="s">
-        <v>30</v>
-      </c>
+      <c r="A8" s="4"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>33</v>
+        <v>16</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="E9" s="7"/>
-      <c r="F9" s="12"/>
+      <c r="F9" s="11" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="12" t="s">
-        <v>37</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="11"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="12"/>
+        <v>16</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="13"/>
+      <c r="F11" s="12" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="5" t="s">
-        <v>44</v>
+        <v>16</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="12" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="8" t="s">
-        <v>48</v>
+        <v>43</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="12" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="15" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="B15" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="C15" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
+      <c r="D15" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="5" t="s">
-        <v>57</v>
+      <c r="E15" s="13"/>
+      <c r="F15" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="E16" s="14"/>
-      <c r="F16" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="A16" s="15"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>15</v>
+        <v>45</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>68</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="16"/>
+      <c r="F20" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="15" t="s">
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="17"/>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="B22" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D22" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="F19" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="12"/>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
+      <c r="E22" s="16"/>
+      <c r="F22" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="B21" s="13" t="s">
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="B23" s="4"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D21" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="E21" s="16"/>
-      <c r="F21" s="18" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="F23" s="5"/>
-    </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="5"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="D25" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>82</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="13"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="12"/>
+      <c r="A26" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="C27" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="D27" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="E27" s="20"/>
-      <c r="F27" s="22" t="s">
-        <v>87</v>
-      </c>
+      <c r="A27" s="12"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="8"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="22"/>
-      <c r="F28" s="22"/>
+      <c r="A28" s="3"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B29" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D29" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4" t="s">
-        <v>92</v>
-      </c>
+      <c r="A29" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="24"/>
+      <c r="A30" s="21"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
-      <c r="D30" s="22"/>
+      <c r="D30" s="4"/>
       <c r="E30" s="4"/>
-      <c r="F30" s="15"/>
+      <c r="F30" s="4"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="25" t="s">
-        <v>93</v>
-      </c>
+      <c r="A31" s="6"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
-      <c r="F31" s="19"/>
+      <c r="E31" s="4"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="25"/>
-      <c r="F32" s="8"/>
+      <c r="A32" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="25" t="s">
+      <c r="A33" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F35" s="14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="D36" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="F36" s="22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="3"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="23"/>
+      <c r="F37" s="22"/>
+    </row>
+    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="F38" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F33" s="15" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="D34" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="F34" s="15" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    </row>
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="3"/>
+      <c r="D39" s="22"/>
+      <c r="F39" s="22"/>
+    </row>
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2056,32 +2069,33 @@
     <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1001" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1002" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1003" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1004" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="D34:D35"/>
+  <mergeCells count="15">
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="F38:F39"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="https://checklists.opquast.com/fr/"/>
-    <hyperlink ref="F4" r:id="rId2" display="https://checklists.opquast.com/fr/"/>
-    <hyperlink ref="F6" r:id="rId3" display="https://www.alsacreations.com/astuce/lire/1562-script-attribut-async-defer.html"/>
-    <hyperlink ref="F8" r:id="rId4" display="https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html"/>
-    <hyperlink ref="F10" r:id="rId5" display="https://www.alsacreations.com/astuce/lire/78-Quelle-est-la-difference-entre-les-chemins-relatifs-et-absolus-.html"/>
-    <hyperlink ref="F12" r:id="rId6" display="    http://www.php-astux.info/chemins-relatif-absolu.php"/>
-    <hyperlink ref="F18" r:id="rId7" display="https://checklists.opquast.com/fr/"/>
-    <hyperlink ref="F27" r:id="rId8" display="https://checklists.opquast.com/fr/"/>
+    <hyperlink ref="F2" r:id="rId1" display="https://checklists.opquast.com/fr/  Règle N°177"/>
+    <hyperlink ref="F7" r:id="rId2" display="https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html"/>
+    <hyperlink ref="F9" r:id="rId3" display="https://www.alsacreations.com/astuce/lire/78-Quelle-est-la-difference-entre-les-chemins-relatifs-et-absolus-.html"/>
+    <hyperlink ref="F11" r:id="rId4" display="    http://www.php-astux.info/chemins-relatif-absolu.php"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>